<commit_message>
feat:(user and major) create management page
</commit_message>
<xml_diff>
--- a/src/seeders/files/xlsx/roles.xlsx
+++ b/src/seeders/files/xlsx/roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phinc\Documents\projects\phincon\personal_project\Project-Akreditasi\src\seeders\files\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1200BC59-53C0-4F1E-A9C8-4E308705B13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF9813A-F07E-49BC-A3F7-E353DE92A684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7110" yWindow="2670" windowWidth="12090" windowHeight="8080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>code</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Study Program</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>Administrator</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -398,12 +404,23 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C4" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix:(notification) enable notification and auto deactive accreditations
</commit_message>
<xml_diff>
--- a/src/seeders/files/xlsx/roles.xlsx
+++ b/src/seeders/files/xlsx/roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phinc\Documents\projects\phincon\personal_project\Project-Akreditasi\src\seeders\files\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF9813A-F07E-49BC-A3F7-E353DE92A684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8823A51-D20A-4B14-A373-B27E934D8F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="2670" windowWidth="12090" windowHeight="8080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>code</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>Study Program</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>Administrator</t>
   </si>
 </sst>
 </file>
@@ -369,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,23 +398,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>